<commit_message>
update statistics for august
</commit_message>
<xml_diff>
--- a/statistics_files/nekls_executive_board/2024/2024_08_next_statistics_for_executive_board.xlsx
+++ b/statistics_files/nekls_executive_board/2024/2024_08_next_statistics_for_executive_board.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\nekls_executive_board\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9442EE69-17C7-4563-826A-7C5DC8A7BC81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA05397-093B-481E-931B-9E4E1ABB34F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21948" windowHeight="8844" xr2:uid="{173C74C7-6DED-436A-89F4-F7E38458C5AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{173C74C7-6DED-436A-89F4-F7E38458C5AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -719,13 +728,13 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" style="22" customWidth="1"/>
-    <col min="2" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" style="22" customWidth="1"/>
+    <col min="2" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +744,7 @@
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -749,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -763,7 +772,7 @@
         <v>7839</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -777,7 +786,7 @@
         <v>3503</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -791,7 +800,7 @@
         <v>6777</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -805,7 +814,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -819,7 +828,7 @@
         <v>6120</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
@@ -833,7 +842,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -847,7 +856,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -861,7 +870,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -875,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
@@ -889,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
@@ -903,7 +912,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
@@ -917,7 +926,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
@@ -931,7 +940,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
@@ -945,7 +954,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
@@ -959,7 +968,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
@@ -973,7 +982,7 @@
         <v>3592</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -987,7 +996,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
@@ -1001,7 +1010,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
@@ -1015,7 +1024,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
@@ -1029,7 +1038,7 @@
         <v>3189</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -1043,7 +1052,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
@@ -1057,7 +1066,7 @@
         <v>3996</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
@@ -1071,7 +1080,7 @@
         <v>9448</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
@@ -1085,7 +1094,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
@@ -1099,7 +1108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>30</v>
       </c>
@@ -1113,7 +1122,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
@@ -1127,7 +1136,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
@@ -1141,7 +1150,7 @@
         <v>3018</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>33</v>
       </c>
@@ -1155,7 +1164,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>34</v>
       </c>
@@ -1169,7 +1178,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
@@ -1183,7 +1192,7 @@
         <v>3131</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
@@ -1197,7 +1206,7 @@
         <v>2248</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
@@ -1211,7 +1220,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>38</v>
       </c>
@@ -1225,7 +1234,7 @@
         <v>5702</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
@@ -1239,7 +1248,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
@@ -1253,7 +1262,7 @@
         <v>2715</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>41</v>
       </c>
@@ -1267,7 +1276,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>42</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>43</v>
       </c>
@@ -1295,7 +1304,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>44</v>
       </c>
@@ -1309,7 +1318,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>45</v>
       </c>
@@ -1323,7 +1332,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>46</v>
       </c>
@@ -1337,7 +1346,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>47</v>
       </c>
@@ -1351,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>48</v>
       </c>
@@ -1365,7 +1374,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>49</v>
       </c>
@@ -1379,7 +1388,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>50</v>
       </c>
@@ -1393,7 +1402,7 @@
         <v>5340</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>51</v>
       </c>
@@ -1407,7 +1416,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>52</v>
       </c>
@@ -1421,7 +1430,7 @@
         <v>2736</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>53</v>
       </c>
@@ -1435,7 +1444,7 @@
         <v>5774</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>54</v>
       </c>
@@ -1449,7 +1458,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>55</v>
       </c>
@@ -1463,7 +1472,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>56</v>
       </c>
@@ -1477,7 +1486,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>57</v>
       </c>
@@ -1491,7 +1500,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>58</v>
       </c>
@@ -1505,7 +1514,7 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>59</v>
       </c>
@@ -1519,7 +1528,7 @@
         <v>2892</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>60</v>
       </c>
@@ -1533,7 +1542,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>61</v>
       </c>

</xml_diff>